<commit_message>
convert razruhlitel to kg
</commit_message>
<xml_diff>
--- a/lab5_6/lab5_6.xlsx
+++ b/lab5_6/lab5_6.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\labs\4.2\ERP\labs\OerpC\ïÉ 5-6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\labs\4.2\ERP\lab5_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="21570" windowHeight="8085" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12315" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Задание" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="ЗаказыКлиентов" sheetId="4" r:id="rId3"/>
     <sheet name="СкладОстатки" sheetId="3" r:id="rId4"/>
     <sheet name="Лабораторная работа №5" sheetId="5" r:id="rId5"/>
+    <sheet name="Лабораторная работа №6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="189">
   <si>
     <t>1.</t>
   </si>
@@ -467,19 +468,196 @@
   </si>
   <si>
     <t>котлеты по киевски + цыпленок</t>
+  </si>
+  <si>
+    <t>Вид оборудования</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Станкоемкость изготовления </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Условного изделия, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>нормо-ч./ед</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Оборудование 1</t>
+  </si>
+  <si>
+    <t>Оборудование 2</t>
+  </si>
+  <si>
+    <t>Оборудование 3</t>
+  </si>
+  <si>
+    <t>Оборудование 4</t>
+  </si>
+  <si>
+    <t>Оборудование 5</t>
+  </si>
+  <si>
+    <t>Оборудование 6</t>
+  </si>
+  <si>
+    <t>Оборудование 7</t>
+  </si>
+  <si>
+    <t>Оборудование</t>
+  </si>
+  <si>
+    <t>Количество оборудования</t>
+  </si>
+  <si>
+    <t>Дано</t>
+  </si>
+  <si>
+    <t>Месяц</t>
+  </si>
+  <si>
+    <t>Июль</t>
+  </si>
+  <si>
+    <t>ПРФ</t>
+  </si>
+  <si>
+    <t>Удельный вес</t>
+  </si>
+  <si>
+    <t>Группа оборудования</t>
+  </si>
+  <si>
+    <t>Количество единиц оборудования (k), шт.</t>
+  </si>
+  <si>
+    <t>Действительный фонд времени единицы оборудования при s-сменном режиме работы (</t>
+  </si>
+  <si>
+    <t>), ч.</t>
+  </si>
+  <si>
+    <t>Действительный фонд времени оборудования (</t>
+  </si>
+  <si>
+    <t>), ч</t>
+  </si>
+  <si>
+    <t>Фк</t>
+  </si>
+  <si>
+    <t>Длительность смены</t>
+  </si>
+  <si>
+    <t>Кол. Раб. Дней</t>
+  </si>
+  <si>
+    <t>Кол. Смен</t>
+  </si>
+  <si>
+    <t>Фпп</t>
+  </si>
+  <si>
+    <t>Кол.
+выходных</t>
+  </si>
+  <si>
+    <t>Кол.нераб
+часов в прзд.</t>
+  </si>
+  <si>
+    <t>Кол. 
+Праздн.
+Дней</t>
+  </si>
+  <si>
+    <t>Кол. Дней</t>
+  </si>
+  <si>
+    <t>Фр</t>
+  </si>
+  <si>
+    <t>Фд</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действительный фонд работы 1 шт. оборудования, ч. </t>
+  </si>
+  <si>
+    <t>Количество единиц оборудования, шт.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пропускная способность , ч. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Норма времени на изготовление единицы условного изделия, нормо-ч./ед. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возможный выпуск - Производственная мощность, шт. </t>
+  </si>
+  <si>
+    <t>Потребность в условном изделии, шт.</t>
+  </si>
+  <si>
+    <t>Цех 1</t>
+  </si>
+  <si>
+    <t>Х</t>
+  </si>
+  <si>
+    <t>Цех 2</t>
+  </si>
+  <si>
+    <t>Цех 3</t>
+  </si>
+  <si>
+    <t>Предприятие</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -506,8 +684,50 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,8 +788,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -668,14 +918,304 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -690,16 +1230,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,7 +1250,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,7 +1261,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -732,10 +1272,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -743,21 +1283,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -769,7 +1309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -778,23 +1318,23 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -805,6 +1345,172 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,6 +1586,274 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>137380</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1062404</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>413605</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1301995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2188918" y="13380793"/>
+          <a:ext cx="276225" cy="239591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>1053245</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>409575</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>1292836</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3078" name="Object 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3078"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>100745</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>1044087</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>996095</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>1283678</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3077" name="Object 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3077"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>201490</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>1172308</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1001590</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>102944</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3076" name="Object 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3076"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100745</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>979976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1234220</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1238617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Рисунок 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8160360" y="13298365"/>
+          <a:ext cx="1133475" cy="258641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -923,7 +1897,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -958,7 +1932,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +3647,9 @@
       <c r="H59" s="4">
         <v>2</v>
       </c>
-      <c r="I59" s="4"/>
+      <c r="I59" s="75">
+        <v>1</v>
+      </c>
       <c r="J59" s="4" t="s">
         <v>108</v>
       </c>
@@ -2703,7 +3679,9 @@
       <c r="H60" s="4">
         <v>2</v>
       </c>
-      <c r="I60" s="4"/>
+      <c r="I60" s="75">
+        <v>1</v>
+      </c>
       <c r="J60" s="4" t="s">
         <v>108</v>
       </c>
@@ -3256,8 +4234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3325,7 +4303,7 @@
         <v>кг</v>
       </c>
       <c r="D4" s="37">
-        <f>СкладОстатки!C3</f>
+        <f>СкладОстатки!$C$3</f>
         <v>10</v>
       </c>
       <c r="E4" s="37">
@@ -3346,7 +4324,7 @@
     </row>
     <row r="5" spans="1:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="38" t="str">
-        <f>ЗаказыКлиентов!B8</f>
+        <f>ЗаказыКлиентов!$B$8</f>
         <v>Цыпленок фаршированный</v>
       </c>
       <c r="C5" s="37" t="str">
@@ -3477,11 +4455,11 @@
         <v>кг</v>
       </c>
       <c r="D12" s="42">
-        <f>СкладОстатки!C12</f>
+        <f>СкладОстатки!$C$12</f>
         <v>10</v>
       </c>
       <c r="E12" s="42">
-        <f>ЗаказыКлиентов!C9</f>
+        <f>ЗаказыКлиентов!$C$9</f>
         <v>50</v>
       </c>
       <c r="F12" s="37">
@@ -3521,11 +4499,11 @@
         <v>кг</v>
       </c>
       <c r="D13" s="54">
-        <f>СкладОстатки!C13</f>
+        <f>СкладОстатки!$C$13</f>
         <v>20</v>
       </c>
       <c r="E13" s="54">
-        <f>ЗаказыКлиентов!C5</f>
+        <f>ЗаказыКлиентов!$C$5</f>
         <v>150</v>
       </c>
       <c r="F13" s="51">
@@ -3540,7 +4518,7 @@
         <v>75.2</v>
       </c>
       <c r="I13" s="53">
-        <f>F4*ОсновныеДанные!C47</f>
+        <f>F4*ОсновныеДанные!$C$47</f>
         <v>376</v>
       </c>
       <c r="J13" s="39"/>
@@ -3565,11 +4543,11 @@
         <v>кг</v>
       </c>
       <c r="D14" s="43">
-        <f>СкладОстатки!C11</f>
+        <f>СкладОстатки!$C$11</f>
         <v>40</v>
       </c>
       <c r="E14" s="43">
-        <f>ЗаказыКлиентов!C6</f>
+        <f>ЗаказыКлиентов!$C$6</f>
         <v>350</v>
       </c>
       <c r="F14" s="56">
@@ -3601,7 +4579,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="45">
-        <f>ЗаказыКлиентов!C7</f>
+        <f>ЗаказыКлиентов!$C$7</f>
         <v>100</v>
       </c>
       <c r="F15" s="56">
@@ -3646,7 +4624,7 @@
         <v>6.4</v>
       </c>
       <c r="I16" s="53">
-        <f>F12*ОсновныеДанные!C54</f>
+        <f>F12*ОсновныеДанные!$C$54</f>
         <v>32</v>
       </c>
       <c r="J16" s="39"/>
@@ -4065,12 +5043,12 @@
       <c r="B33" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="37" t="s">
-        <v>28</v>
+      <c r="C33" s="116" t="s">
+        <v>5</v>
       </c>
       <c r="D33" s="45">
-        <f>СкладОстатки!C27</f>
-        <v>90</v>
+        <f>СкладОстатки!C27/1000</f>
+        <v>0.09</v>
       </c>
       <c r="E33" s="38">
         <v>0</v>
@@ -4080,7 +5058,7 @@
       </c>
       <c r="G33" s="37">
         <f t="shared" si="2"/>
-        <v>-89.850239999999999</v>
+        <v>5.9760000000000001E-2</v>
       </c>
       <c r="H33" s="37">
         <f>I33*СкладОстатки!$E$32</f>
@@ -4358,4 +5336,1057 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A46" zoomScale="104" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="61"/>
+      <c r="E2" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="78" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="66">
+        <v>2</v>
+      </c>
+      <c r="D3" s="61"/>
+      <c r="E3" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="70">
+        <v>0.15</v>
+      </c>
+      <c r="G3" s="70">
+        <v>8</v>
+      </c>
+      <c r="H3" s="70">
+        <v>5</v>
+      </c>
+      <c r="I3" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="68">
+        <v>4</v>
+      </c>
+      <c r="D4" s="61"/>
+    </row>
+    <row r="5" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="68">
+        <v>6</v>
+      </c>
+      <c r="D5" s="62"/>
+    </row>
+    <row r="6" spans="1:25" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="68">
+        <v>5</v>
+      </c>
+      <c r="D6" s="62"/>
+    </row>
+    <row r="7" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="68">
+        <v>3</v>
+      </c>
+      <c r="D7" s="62"/>
+    </row>
+    <row r="8" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="68">
+        <v>2</v>
+      </c>
+      <c r="D8" s="62"/>
+    </row>
+    <row r="9" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="70">
+        <v>2</v>
+      </c>
+      <c r="D9" s="62"/>
+    </row>
+    <row r="10" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="62"/>
+    </row>
+    <row r="11" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" s="74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="37">
+        <f>'Лабораторная работа №5'!F4</f>
+        <v>470</v>
+      </c>
+      <c r="I16" s="38">
+        <f>H16/SUM(H16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="38" t="str">
+        <f>ЗаказыКлиентов!$B$8</f>
+        <v>Цыпленок фаршированный</v>
+      </c>
+      <c r="H17" s="37">
+        <f>'Лабораторная работа №5'!F5</f>
+        <v>120</v>
+      </c>
+      <c r="I17" s="38">
+        <f>H17/SUM(H17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="38" t="str">
+        <f>'Лабораторная работа №5'!B12</f>
+        <v>Блины</v>
+      </c>
+      <c r="H18" s="37">
+        <f>'Лабораторная работа №5'!F12</f>
+        <v>40</v>
+      </c>
+      <c r="I18" s="38">
+        <f>H18/SUM(H18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="38" t="str">
+        <f>'Лабораторная работа №5'!B13</f>
+        <v>Фарш куриный</v>
+      </c>
+      <c r="H19" s="37">
+        <f>'Лабораторная работа №5'!F13</f>
+        <v>581.20000000000005</v>
+      </c>
+      <c r="I19" s="38">
+        <f>H19/SUM(H19:H21)</f>
+        <v>0.58635996771589993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="84"/>
+      <c r="C20" s="84"/>
+      <c r="G20" s="38" t="str">
+        <f>'Лабораторная работа №5'!B14</f>
+        <v>Фарш домашний</v>
+      </c>
+      <c r="H20" s="37">
+        <f>'Лабораторная работа №5'!F14</f>
+        <v>310</v>
+      </c>
+      <c r="I20" s="38">
+        <f>H20/SUM(H19:H21)</f>
+        <v>0.31275221953188054</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="85"/>
+      <c r="C21" s="85"/>
+      <c r="G21" s="38" t="str">
+        <f>'Лабораторная работа №5'!B15</f>
+        <v>Фарш говяжий</v>
+      </c>
+      <c r="H21" s="37">
+        <f>'Лабораторная работа №5'!F15</f>
+        <v>100</v>
+      </c>
+      <c r="I21" s="38">
+        <f>H21/SUM(H19:H21)</f>
+        <v>0.10088781275221953</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="73">
+        <f>SUM(I19*ОсновныеДанные!I22,I20*ОсновныеДанные!I13,I21*ОсновныеДанные!I4)/100</f>
+        <v>4.4136400322840996E-2</v>
+      </c>
+      <c r="G22" s="38" t="str">
+        <f>'Лабораторная работа №5'!B16</f>
+        <v>Тесто</v>
+      </c>
+      <c r="H22" s="37">
+        <f>'Лабораторная работа №5'!F16</f>
+        <v>38.4</v>
+      </c>
+      <c r="I22" s="38">
+        <f>H22/SUM(H22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="73">
+        <f>SUM(I19*ОсновныеДанные!I23,I20*ОсновныеДанные!I14,I21*ОсновныеДанные!I5)/100</f>
+        <v>1.7068200161420501E-2</v>
+      </c>
+      <c r="K23" s="55"/>
+    </row>
+    <row r="24" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="73">
+        <f>I22*ОсновныеДанные!I30/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="73">
+        <f>I16*ОсновныеДанные!I47/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="73">
+        <f>I16*ОсновныеДанные!I49/10</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="73">
+        <f>I18*ОсновныеДанные!I54/10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="73">
+        <f>SUM('Лабораторная работа №6'!I17*ОсновныеДанные!I59,'Лабораторная работа №6'!I17*ОсновныеДанные!I59)/10</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="31"/>
+      <c r="Y31" s="31"/>
+    </row>
+    <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:25" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="83" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="86" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" s="86" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="H36" s="79" t="s">
+        <v>167</v>
+      </c>
+      <c r="I36" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="K36" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="L36" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="M36" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="N36" s="82" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="38">
+        <v>31</v>
+      </c>
+      <c r="H37" s="37">
+        <f>31*24</f>
+        <v>744</v>
+      </c>
+      <c r="I37" s="38">
+        <f>H37*F3</f>
+        <v>111.6</v>
+      </c>
+      <c r="J37" s="37">
+        <v>9</v>
+      </c>
+      <c r="K37" s="38">
+        <v>0</v>
+      </c>
+      <c r="L37" s="37">
+        <v>0</v>
+      </c>
+      <c r="M37" s="81">
+        <f>$G$3*($G$37-$J$37-$L$37)</f>
+        <v>176</v>
+      </c>
+      <c r="N37" s="32">
+        <f>M37-I37</f>
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="73">
+        <f>C3</f>
+        <v>2</v>
+      </c>
+      <c r="D38" s="65">
+        <f>$N$37</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E38" s="66">
+        <f>D38*C38</f>
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="73">
+        <f t="shared" ref="C39:C44" si="0">C4</f>
+        <v>4</v>
+      </c>
+      <c r="D39" s="65">
+        <f t="shared" ref="D39:D44" si="1">$N$37</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E39" s="66">
+        <f t="shared" ref="E39:E44" si="2">D39*C39</f>
+        <v>257.60000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="73">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D40" s="65">
+        <f t="shared" si="1"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E40" s="66">
+        <f t="shared" si="2"/>
+        <v>386.40000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="73">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D41" s="65">
+        <f t="shared" si="1"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E41" s="66">
+        <f t="shared" si="2"/>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="81">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D42" s="65">
+        <f t="shared" si="1"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E42" s="66">
+        <f t="shared" si="2"/>
+        <v>193.20000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="73">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D43" s="65">
+        <f t="shared" si="1"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E43" s="66">
+        <f t="shared" si="2"/>
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="73">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D44" s="65">
+        <f t="shared" si="1"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E44" s="66">
+        <f t="shared" si="2"/>
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31"/>
+      <c r="Y47" s="31"/>
+    </row>
+    <row r="48" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="2:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="89" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="90" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="E49" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="G49" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="H49" s="91" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="92"/>
+      <c r="C50" s="88"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="99"/>
+      <c r="F50" s="88"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="93"/>
+    </row>
+    <row r="51" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="94" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" s="100">
+        <f>D38</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D51" s="101">
+        <f>C38</f>
+        <v>2</v>
+      </c>
+      <c r="E51" s="102">
+        <f>D51*C51</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F51" s="100">
+        <f>C22</f>
+        <v>4.4136400322840996E-2</v>
+      </c>
+      <c r="G51" s="100">
+        <f>E51/F51</f>
+        <v>2918.2262046264977</v>
+      </c>
+      <c r="H51" s="103">
+        <f>SUM(H$19:H$21)</f>
+        <v>991.2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="95" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" s="104">
+        <f>D39</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D52" s="105">
+        <f>C39</f>
+        <v>4</v>
+      </c>
+      <c r="E52" s="102">
+        <f>D52*C52</f>
+        <v>257.60000000000002</v>
+      </c>
+      <c r="F52" s="102">
+        <f>C23</f>
+        <v>1.7068200161420501E-2</v>
+      </c>
+      <c r="G52" s="102">
+        <f>E52/F52</f>
+        <v>15092.393899988179</v>
+      </c>
+      <c r="H52" s="102">
+        <f>SUM(H$19:H$21)</f>
+        <v>991.2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="112">
+        <f>MIN(E51:E52)</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F53" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="H53" s="106" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="97"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="109"/>
+    </row>
+    <row r="55" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="96" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="106">
+        <f>D40</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D55" s="106">
+        <f>C40</f>
+        <v>6</v>
+      </c>
+      <c r="E55" s="106">
+        <f>C55*D55</f>
+        <v>386.40000000000003</v>
+      </c>
+      <c r="F55" s="110">
+        <f>C24</f>
+        <v>0.2</v>
+      </c>
+      <c r="G55" s="102">
+        <f>E55/F55</f>
+        <v>1932</v>
+      </c>
+      <c r="H55" s="114">
+        <f>'Лабораторная работа №6'!H22</f>
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="96" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" s="112">
+        <f>E55</f>
+        <v>386.40000000000003</v>
+      </c>
+      <c r="F56" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="G56" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="H56" s="106" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="97"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="108"/>
+      <c r="F57" s="108"/>
+      <c r="G57" s="108"/>
+      <c r="H57" s="109"/>
+    </row>
+    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="96" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="106">
+        <f>D41</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D58" s="106">
+        <f>C41</f>
+        <v>5</v>
+      </c>
+      <c r="E58" s="106">
+        <f>C58*D58</f>
+        <v>322</v>
+      </c>
+      <c r="F58" s="106">
+        <f>C25</f>
+        <v>0.1</v>
+      </c>
+      <c r="G58" s="100">
+        <f>E58/F58</f>
+        <v>3220</v>
+      </c>
+      <c r="H58" s="107">
+        <f>H16</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="106">
+        <f t="shared" ref="C59:C61" si="3">D42</f>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D59" s="106">
+        <f t="shared" ref="D59:D61" si="4">C42</f>
+        <v>3</v>
+      </c>
+      <c r="E59" s="106">
+        <f t="shared" ref="E59:E61" si="5">C59*D59</f>
+        <v>193.20000000000002</v>
+      </c>
+      <c r="F59" s="110">
+        <f t="shared" ref="F59:F61" si="6">C26</f>
+        <v>0.3</v>
+      </c>
+      <c r="G59" s="115">
+        <f t="shared" ref="G59:G61" si="7">E59/F59</f>
+        <v>644.00000000000011</v>
+      </c>
+      <c r="H59" s="107">
+        <f>H58</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="106">
+        <f t="shared" si="3"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D60" s="106">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E60" s="106">
+        <f t="shared" si="5"/>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F60" s="106">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="G60" s="100">
+        <f t="shared" si="7"/>
+        <v>1288</v>
+      </c>
+      <c r="H60" s="107">
+        <f>H18</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="106">
+        <f t="shared" si="3"/>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D61" s="106">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="106">
+        <f t="shared" si="5"/>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F61" s="110">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="G61" s="115">
+        <f t="shared" si="7"/>
+        <v>644</v>
+      </c>
+      <c r="H61" s="107">
+        <f>H17</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D62" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" s="112">
+        <f>MIN(E58:E61)</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F62" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="G62" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="H62" s="107" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="97"/>
+      <c r="C63" s="108"/>
+      <c r="D63" s="108"/>
+      <c r="E63" s="108"/>
+      <c r="F63" s="108"/>
+      <c r="G63" s="108"/>
+      <c r="H63" s="109"/>
+    </row>
+    <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="98" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="E64" s="113">
+        <f>MIN(E62,E56,E53)</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F64" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="G64" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="H64" s="107" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="3078" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>1057275</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>409575</xdr:colOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>1295400</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="3078" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="3077" r:id="rId6">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>1047750</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1000125</xdr:colOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>1285875</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="3077" r:id="rId6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="3076" r:id="rId8">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>48</xdr:row>
+                <xdr:rowOff>1171575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1000125</xdr:colOff>
+                <xdr:row>49</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="3076" r:id="rId8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
+</worksheet>
 </file>
</xml_diff>